<commit_message>
Fixed workbook and removed propane.
</commit_message>
<xml_diff>
--- a/Workbook1.xlsx
+++ b/Workbook1.xlsx
@@ -1,16 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr showInkAnnotation="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusuf/Documents/FYDP/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94079E3E-A383-644D-ADD5-713EB91847C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8052" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28420" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Species</t>
   </si>
@@ -27,9 +38,6 @@
     <t>Carbon Dioxide</t>
   </si>
   <si>
-    <t>Propane</t>
-  </si>
-  <si>
     <t>Membrane Periabilities [cm^3 (STP) cm/(cm^2 s atm)]</t>
   </si>
   <si>
@@ -55,12 +63,6 @@
   </si>
   <si>
     <t>Paper</t>
-  </si>
-  <si>
-    <t>Isopentyl Acetate</t>
-  </si>
-  <si>
-    <t>1-s2.0-S0376738808005504-main.pdf</t>
   </si>
   <si>
     <t>Acetaldehyde</t>
@@ -75,8 +77,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -383,58 +385,58 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="96.9" customHeight="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -463,27 +465,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1.6884594778660613E-9</v>
       </c>
       <c r="C3" s="2">
-        <v>5.2999999999999996E-13</v>
+        <v>1.35E-11</v>
       </c>
       <c r="D3">
-        <v>4.4000000000000004</v>
+        <f>20/1000</f>
+        <v>0.02</v>
       </c>
       <c r="E3">
-        <v>95.1</v>
+        <v>740</v>
       </c>
       <c r="F3" s="2">
-        <v>5.4999999999999997E-3</v>
+        <f>1/14*1.01*1000/G3</f>
+        <v>1.6376377804657376E-3</v>
       </c>
       <c r="G3" s="2">
-        <v>44100</v>
+        <v>44053</v>
       </c>
       <c r="H3" s="2">
         <v>0</v>
@@ -491,97 +495,42 @@
       <c r="I3" s="2">
         <v>0</v>
       </c>
+      <c r="J3" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2">
-        <v>4.8320000000000001E-11</v>
+      <c r="B4">
+        <v>1.3934008326394671E-9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>8.7099999999999998E-12</v>
+      </c>
+      <c r="D4">
+        <f>400/1000</f>
+        <v>0.4</v>
       </c>
       <c r="E4">
-        <f>0.3095*760</f>
-        <v>235.22</v>
+        <v>16.22</v>
+      </c>
+      <c r="F4" s="2">
+        <f>1/5000*1.01*1000/G4</f>
+        <v>3.3637514154399522E-6</v>
       </c>
       <c r="G4" s="2">
-        <v>139190</v>
-      </c>
-      <c r="H4">
+        <v>60052</v>
+      </c>
+      <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>0</v>
       </c>
       <c r="J4" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>1.6884594778660613E-9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.35E-11</v>
-      </c>
-      <c r="D5">
-        <f>20/1000</f>
-        <v>0.02</v>
-      </c>
-      <c r="E5">
-        <v>740</v>
-      </c>
-      <c r="F5" s="2">
-        <f>1/14*1.01*1000/G5</f>
-        <v>1.6376377804657376E-3</v>
-      </c>
-      <c r="G5" s="2">
-        <v>44053</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>1.3934008326394671E-9</v>
-      </c>
-      <c r="C6" s="2">
-        <v>8.7099999999999998E-12</v>
-      </c>
-      <c r="D6">
-        <f>400/1000</f>
-        <v>0.4</v>
-      </c>
-      <c r="E6">
-        <v>16.22</v>
-      </c>
-      <c r="F6" s="2">
-        <f>1/5000*1.01*1000/G6</f>
-        <v>3.3637514154399522E-6</v>
-      </c>
-      <c r="G6" s="2">
-        <v>60052</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve plot of CrankFitting
</commit_message>
<xml_diff>
--- a/Workbook1.xlsx
+++ b/Workbook1.xlsx
@@ -1,27 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusuf/Documents/FYDP/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94079E3E-A383-644D-ADD5-713EB91847C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28420" windowHeight="15920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8052" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Species</t>
   </si>
@@ -72,13 +61,34 @@
   </si>
   <si>
     <t>Release Kinetics of Volatile Organic Compounds from Roasted and Ground Coffee: Online Measurements by PTR-MS and Mathematical Modeling</t>
+  </si>
+  <si>
+    <t>Hexanal</t>
+  </si>
+  <si>
+    <t>2-methylbutanal</t>
+  </si>
+  <si>
+    <t>2-methylpropanal</t>
+  </si>
+  <si>
+    <t>Investigation of roasted coffee freshness with an improved headspace technique</t>
+  </si>
+  <si>
+    <t>Coffee roasting and quenching technology -formation and stability of aroma compounds</t>
+  </si>
+  <si>
+    <t>Pyridine</t>
+  </si>
+  <si>
+    <t>Approximate permeation as benzene</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,12 +97,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,12 +123,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,26 +403,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="96.9" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,7 +454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -465,7 +483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -476,8 +494,7 @@
         <v>1.35E-11</v>
       </c>
       <c r="D3">
-        <f>20/1000</f>
-        <v>0.02</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="E3">
         <v>740</v>
@@ -499,7 +516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -531,6 +548,134 @@
       </c>
       <c r="J4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>2.796E-10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>5.5570000000000001E-8</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5.1900000000000004E-4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>100.161</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="16.2" customHeight="1">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>5.5799999999999997E-8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4.7027000000000001E-8</v>
+      </c>
+      <c r="D6">
+        <v>2.07E-2</v>
+      </c>
+      <c r="E6">
+        <v>49.317000999999998</v>
+      </c>
+      <c r="F6" s="2">
+        <v>4.9346000000000004E-4</v>
+      </c>
+      <c r="G6" s="2">
+        <v>86.134</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>2.4E-8</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.5424E-8</v>
+      </c>
+      <c r="D7">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>170</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.9699999999999999E-4</v>
+      </c>
+      <c r="G7" s="2">
+        <v>72.058000000000007</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>4.8208374409751881E-8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8.7099999999999998E-12</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.3E-3</v>
+      </c>
+      <c r="E8">
+        <v>20.8</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1.1E-5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>79.102000000000004</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>